<commit_message>
updates from pascale and feather team
</commit_message>
<xml_diff>
--- a/data-raw/metadata/feather_mini_snorkel_metadata.xlsx
+++ b/data-raw/metadata/feather_mini_snorkel_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashleyvizek/code/feather-mini-snorkel/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFEBB9EA-845B-D342-B11E-6B0738D3FF52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EE29965-7F3C-4644-ABB3-E1429A691C70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="61740" yWindow="520" windowWidth="30680" windowHeight="22840" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="63660" yWindow="3400" windowWidth="30680" windowHeight="22840" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dataset" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="77">
   <si>
     <t>name</t>
   </si>
@@ -250,7 +250,16 @@
     <t>cover</t>
   </si>
   <si>
-    <t>HR&amp;L</t>
+    <t>tule perch</t>
+  </si>
+  <si>
+    <t>speckled dace</t>
+  </si>
+  <si>
+    <t>sacramento pikeminnow</t>
+  </si>
+  <si>
+    <t>Healthy Rivers and Landscapes</t>
   </si>
 </sst>
 </file>
@@ -822,13 +831,16 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="25.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -885,7 +897,22 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>73</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -995,9 +1022,11 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M23" sqref="M23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -1019,6 +1048,11 @@
       </c>
       <c r="F1" t="s">
         <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adds attachments and md for methods
</commit_message>
<xml_diff>
--- a/data-raw/metadata/feather_mini_snorkel_metadata.xlsx
+++ b/data-raw/metadata/feather_mini_snorkel_metadata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashleyvizek/code/feather-mini-snorkel/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EE29965-7F3C-4644-ABB3-E1429A691C70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{109FA140-97F7-6246-8202-D289EC01316C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="63660" yWindow="3400" windowWidth="30680" windowHeight="22840" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="78">
   <si>
     <t>name</t>
   </si>
@@ -260,6 +260,9 @@
   </si>
   <si>
     <t>Healthy Rivers and Landscapes</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
@@ -1025,7 +1028,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M23" sqref="M23"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1053,6 +1056,15 @@
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D2" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updates project metadata max date
</commit_message>
<xml_diff>
--- a/data-raw/metadata/feather_mini_snorkel_metadata.xlsx
+++ b/data-raw/metadata/feather_mini_snorkel_metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashleyvizek/code/feather-mini-snorkel/data-raw/metadata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Badhia\Documents\git\feather-mini-snorkel\data-raw\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E154D4F-38E6-534C-A3F8-54B624B56E13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6D6DD8C-B642-4451-8098-9C6D5A16227D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="63660" yWindow="3400" windowWidth="30680" windowHeight="22840" firstSheet="1" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-27600" yWindow="1335" windowWidth="20595" windowHeight="13275" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dataset" sheetId="1" r:id="rId1"/>
@@ -669,9 +669,9 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -682,7 +682,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>57</v>
       </c>
@@ -700,13 +700,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>40</v>
       </c>
@@ -738,12 +738,12 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>71</v>
       </c>
@@ -769,7 +769,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>75</v>
       </c>
@@ -795,7 +795,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>70</v>
       </c>
@@ -835,9 +835,9 @@
       <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -857,7 +857,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>53</v>
       </c>
@@ -874,7 +874,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>63</v>
       </c>
@@ -905,9 +905,9 @@
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -915,7 +915,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>62</v>
       </c>
@@ -937,12 +937,12 @@
       <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.33203125" customWidth="1"/>
+    <col min="1" max="1" width="25.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>13</v>
       </c>
@@ -950,67 +950,67 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>72</v>
       </c>
@@ -1029,9 +1029,9 @@
       <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -1048,7 +1048,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>61</v>
       </c>
@@ -1072,9 +1072,9 @@
       <selection activeCell="J38" sqref="J38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -1094,7 +1094,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>53</v>
       </c>
@@ -1128,9 +1128,9 @@
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>25</v>
       </c>
@@ -1150,7 +1150,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -1178,9 +1178,9 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>31</v>
       </c>
@@ -1188,7 +1188,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>59</v>
       </c>
@@ -1203,16 +1203,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="6" max="7" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="17.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>33</v>
       </c>
@@ -1235,7 +1235,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>58</v>
       </c>
@@ -1255,7 +1255,7 @@
         <v>36963</v>
       </c>
       <c r="G2" s="1">
-        <v>37125</v>
+        <v>37488</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
checks metadata, creates xml
</commit_message>
<xml_diff>
--- a/data-raw/metadata/feather_mini_snorkel_metadata.xlsx
+++ b/data-raw/metadata/feather_mini_snorkel_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Badhia\Documents\git\feather-mini-snorkel\data-raw\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6D6DD8C-B642-4451-8098-9C6D5A16227D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CD646F6-812C-4C5E-9AD8-6FCC0F7CDD08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27600" yWindow="1335" windowWidth="20595" windowHeight="13275" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-26730" yWindow="1890" windowWidth="21945" windowHeight="11760" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dataset" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="90">
   <si>
     <t>name</t>
   </si>
@@ -121,9 +121,6 @@
     <t>award_url</t>
   </si>
   <si>
-    <t>funding_description</t>
-  </si>
-  <si>
     <t>status</t>
   </si>
   <si>
@@ -253,55 +250,55 @@
     <t>Healthy Rivers and Landscapes</t>
   </si>
   <si>
+    <t xml:space="preserve">steelhead trout </t>
+  </si>
+  <si>
+    <t>Rhinichthys</t>
+  </si>
+  <si>
+    <t>osculus</t>
+  </si>
+  <si>
+    <t>Oncorhynchus</t>
+  </si>
+  <si>
+    <t>mykiss</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hysterocarpus </t>
+  </si>
+  <si>
+    <t xml:space="preserve">traskii </t>
+  </si>
+  <si>
+    <t>Animalia</t>
+  </si>
+  <si>
+    <t>Chordata</t>
+  </si>
+  <si>
+    <t>Actinopterygii</t>
+  </si>
+  <si>
+    <t>Cypriniformes</t>
+  </si>
+  <si>
+    <t>Cyprinidae</t>
+  </si>
+  <si>
+    <t>Salmoniformes</t>
+  </si>
+  <si>
+    <t>Salmonidae</t>
+  </si>
+  <si>
+    <t>Embiotocidae</t>
+  </si>
+  <si>
+    <t>Perciformes</t>
+  </si>
+  <si>
     <t>NA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">steelhead trout </t>
-  </si>
-  <si>
-    <t>Rhinichthys</t>
-  </si>
-  <si>
-    <t>osculus</t>
-  </si>
-  <si>
-    <t>Oncorhynchus</t>
-  </si>
-  <si>
-    <t>mykiss</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hysterocarpus </t>
-  </si>
-  <si>
-    <t xml:space="preserve">traskii </t>
-  </si>
-  <si>
-    <t>Animalia</t>
-  </si>
-  <si>
-    <t>Chordata</t>
-  </si>
-  <si>
-    <t>Actinopterygii</t>
-  </si>
-  <si>
-    <t>Cypriniformes</t>
-  </si>
-  <si>
-    <t>Cyprinidae</t>
-  </si>
-  <si>
-    <t>Salmoniformes</t>
-  </si>
-  <si>
-    <t>Salmonidae</t>
-  </si>
-  <si>
-    <t>Embiotocidae</t>
-  </si>
-  <si>
-    <t>Perciformes</t>
   </si>
 </sst>
 </file>
@@ -684,7 +681,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
@@ -708,117 +705,117 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" t="s">
         <v>40</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>41</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>42</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>43</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>44</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>45</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>46</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>47</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>48</v>
-      </c>
-      <c r="J1" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D3" t="s">
+        <v>81</v>
+      </c>
+      <c r="E3" t="s">
         <v>82</v>
       </c>
-      <c r="D3" t="s">
+      <c r="F3" t="s">
         <v>83</v>
       </c>
-      <c r="E3" t="s">
+      <c r="G3" t="s">
         <v>84</v>
       </c>
-      <c r="F3" t="s">
-        <v>85</v>
-      </c>
-      <c r="G3" t="s">
-        <v>86</v>
-      </c>
       <c r="H3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="I3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D4" t="s">
+        <v>81</v>
+      </c>
+      <c r="E4" t="s">
         <v>82</v>
       </c>
-      <c r="D4" t="s">
-        <v>83</v>
-      </c>
-      <c r="E4" t="s">
-        <v>84</v>
-      </c>
       <c r="F4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="H4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C5" t="s">
+        <v>80</v>
+      </c>
+      <c r="D5" t="s">
+        <v>81</v>
+      </c>
+      <c r="E5" t="s">
         <v>82</v>
       </c>
-      <c r="D5" t="s">
-        <v>83</v>
-      </c>
-      <c r="E5" t="s">
-        <v>84</v>
-      </c>
       <c r="F5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="G5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="I5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -859,16 +856,16 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E2" t="s">
         <v>10</v>
@@ -876,19 +873,19 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C3" t="s">
         <v>63</v>
       </c>
-      <c r="B3" t="s">
+      <c r="D3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E3" t="s">
         <v>66</v>
-      </c>
-      <c r="C3" t="s">
-        <v>64</v>
-      </c>
-      <c r="D3" t="s">
-        <v>65</v>
-      </c>
-      <c r="E3" t="s">
-        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -917,10 +914,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -977,42 +974,42 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -1050,7 +1047,7 @@
     </row>
     <row r="2" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1096,16 +1093,16 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>54</v>
-      </c>
       <c r="D2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E2" t="s">
         <v>10</v>
@@ -1122,15 +1119,18 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="6" max="6" width="18.90625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>25</v>
       </c>
@@ -1146,22 +1146,19 @@
       <c r="E1" t="s">
         <v>29</v>
       </c>
-      <c r="F1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>74</v>
+        <v>89</v>
       </c>
       <c r="C2" t="s">
-        <v>74</v>
+        <v>89</v>
       </c>
       <c r="D2" t="s">
-        <v>74</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -1182,15 +1179,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" t="s">
         <v>31</v>
-      </c>
-      <c r="B1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -1203,7 +1200,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
@@ -1214,30 +1211,30 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" t="s">
         <v>33</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>34</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>35</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>36</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>37</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>38</v>
-      </c>
-      <c r="G1" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B2">
         <v>-121.63263600000001</v>

</xml_diff>